<commit_message>
bugfix for config file
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingLevelUp.xlsx
+++ b/gameData/shared/BuildingLevelUp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-260" yWindow="1480" windowWidth="37240" windowHeight="17680" tabRatio="883" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="883" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="keep" sheetId="17" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="barracks" sheetId="32" r:id="rId8"/>
     <sheet name="armyCamp" sheetId="33" r:id="rId9"/>
     <sheet name="blackSmith" sheetId="34" r:id="rId10"/>
-    <sheet name="materiarDepot" sheetId="35" r:id="rId11"/>
+    <sheet name="materialDepot" sheetId="35" r:id="rId11"/>
     <sheet name="toolShop" sheetId="36" r:id="rId12"/>
     <sheet name="lumbermill" sheetId="27" r:id="rId13"/>
     <sheet name="stonemason" sheetId="28" r:id="rId14"/>
@@ -2750,8 +2750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -13618,7 +13618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>

</xml_diff>